<commit_message>
Robot V4 - Green
Version V4 is now complete.
</commit_message>
<xml_diff>
--- a/Green/RobotV4_BOM.xlsx
+++ b/Green/RobotV4_BOM.xlsx
@@ -43,9 +43,6 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>Zahnriemen T5 - Z80  - L510mm</t>
-  </si>
-  <si>
     <t>Rubber</t>
   </si>
   <si>
@@ -449,6 +446,9 @@
   </si>
   <si>
     <t>DIN 934 - M3</t>
+  </si>
+  <si>
+    <t>Zahnriemen T5 - Z102  - L510mm</t>
   </si>
 </sst>
 </file>
@@ -3666,7 +3666,7 @@
   <dimension ref="A1:G89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3707,35 +3707,35 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3"/>
     </row>
@@ -3745,35 +3745,35 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4"/>
     </row>
     <row r="5" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5"/>
     </row>
@@ -3783,35 +3783,35 @@
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7"/>
     </row>
@@ -3821,54 +3821,54 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8"/>
     </row>
     <row r="9" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9"/>
     </row>
     <row r="10" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10"/>
     </row>
@@ -3878,16 +3878,16 @@
         <v>6</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11"/>
     </row>
@@ -3897,16 +3897,16 @@
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12"/>
     </row>
@@ -3916,16 +3916,16 @@
         <v>6</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="F13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13"/>
     </row>
@@ -3935,16 +3935,16 @@
         <v>6</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="F14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14"/>
     </row>
@@ -3954,16 +3954,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="F15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15"/>
     </row>
@@ -3973,54 +3973,54 @@
         <v>6</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="F16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16"/>
     </row>
     <row r="17" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="E17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G18"/>
     </row>
@@ -4030,73 +4030,73 @@
         <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G20"/>
     </row>
     <row r="21" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G21"/>
     </row>
     <row r="22" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G22"/>
     </row>
@@ -4106,111 +4106,111 @@
         <v>6</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="E24" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="E26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G26"/>
     </row>
     <row r="27" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28"/>
     </row>
@@ -4220,548 +4220,548 @@
         <v>6</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G30"/>
     </row>
     <row r="31" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="D33" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="E34" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="D36" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3"/>
       <c r="B40" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="D41" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G41"/>
     </row>
     <row r="42" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>49</v>
-      </c>
       <c r="E43" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="E44" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G44"/>
     </row>
     <row r="45" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G46"/>
     </row>
     <row r="47" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E47" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G48"/>
     </row>
     <row r="49" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="F49" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G49"/>
     </row>
     <row r="50" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="D50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="F50" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G50"/>
     </row>
     <row r="51" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="F51" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G51"/>
     </row>
     <row r="52" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="D52" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="F52" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G52"/>
     </row>
     <row r="53" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="F53" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G53"/>
     </row>
     <row r="54" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C54" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="E54" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G54"/>
     </row>
     <row r="55" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3"/>
       <c r="B55" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="D55" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G55"/>
     </row>
     <row r="56" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3"/>
       <c r="B56" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G56"/>
     </row>
     <row r="57" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G57"/>
     </row>
@@ -4771,16 +4771,16 @@
         <v>6</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G58"/>
     </row>
@@ -4790,13 +4790,13 @@
         <v>6</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>8</v>
@@ -4809,13 +4809,13 @@
         <v>6</v>
       </c>
       <c r="C60" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="E60" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>8</v>
@@ -4828,13 +4828,13 @@
         <v>6</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>8</v>
@@ -4847,13 +4847,13 @@
         <v>6</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>8</v>
@@ -4863,16 +4863,16 @@
     <row r="63" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>8</v>
@@ -4885,13 +4885,13 @@
         <v>6</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>8</v>
@@ -4904,13 +4904,13 @@
         <v>6</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>8</v>
@@ -4923,13 +4923,13 @@
         <v>6</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>8</v>
@@ -4942,13 +4942,13 @@
         <v>6</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>8</v>
@@ -4961,13 +4961,13 @@
         <v>6</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D68" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>8</v>
@@ -4980,13 +4980,13 @@
         <v>6</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>8</v>
@@ -4999,13 +4999,13 @@
         <v>6</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>8</v>
@@ -5018,13 +5018,13 @@
         <v>6</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>8</v>
@@ -5037,13 +5037,13 @@
         <v>6</v>
       </c>
       <c r="C72" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="E72" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>8</v>
@@ -5056,13 +5056,13 @@
         <v>6</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>8</v>
@@ -5075,13 +5075,13 @@
         <v>6</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>8</v>
@@ -5094,13 +5094,13 @@
         <v>6</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>8</v>
@@ -5113,13 +5113,13 @@
         <v>6</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>8</v>
@@ -5132,13 +5132,13 @@
         <v>6</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>8</v>
@@ -5151,13 +5151,13 @@
         <v>6</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>8</v>
@@ -5170,13 +5170,13 @@
         <v>6</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>8</v>
@@ -5186,16 +5186,16 @@
     <row r="80" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
       <c r="B80" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>8</v>
@@ -5205,16 +5205,16 @@
     <row r="81" spans="1:7" ht="99.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3"/>
       <c r="B81" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>8</v>
@@ -5227,13 +5227,13 @@
         <v>6</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>8</v>
@@ -5246,13 +5246,13 @@
         <v>6</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>8</v>
@@ -5265,13 +5265,13 @@
         <v>6</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>8</v>
@@ -5284,13 +5284,13 @@
         <v>6</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>8</v>
@@ -5303,13 +5303,13 @@
         <v>6</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>8</v>
@@ -5322,13 +5322,13 @@
         <v>6</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>8</v>
@@ -5341,13 +5341,13 @@
         <v>6</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Adding English translation sheet for v4 BOM spreadsheet
</commit_message>
<xml_diff>
--- a/Green/RobotV4_BOM.xlsx
+++ b/Green/RobotV4_BOM.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\d\BetaBots-Robot-Arm-Project\Green\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="14640"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="14640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
+    <sheet name="Part List (English)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="354">
   <si>
     <t>Bauteilnummer</t>
   </si>
@@ -938,16 +944,165 @@
   </si>
   <si>
     <t>0,284 kg</t>
+  </si>
+  <si>
+    <t>Part Name</t>
+  </si>
+  <si>
+    <t>BOM Type</t>
+  </si>
+  <si>
+    <t>Purchased</t>
+  </si>
+  <si>
+    <t>ABS Plastic</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>Austenitic stainless steel</t>
+  </si>
+  <si>
+    <t>Stainless steel</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Estimated Cost</t>
+  </si>
+  <si>
+    <t>Mass (kg)</t>
+  </si>
+  <si>
+    <t>Brass</t>
+  </si>
+  <si>
+    <t>Nickel-Copper Alloy</t>
+  </si>
+  <si>
+    <t>Clear polycarbonate</t>
+  </si>
+  <si>
+    <t>Carbon steel</t>
+  </si>
+  <si>
+    <t>Spring-type straight pins -- Slotted, light duty</t>
+  </si>
+  <si>
+    <t>Hex socket head screw</t>
+  </si>
+  <si>
+    <t>Washer</t>
+  </si>
+  <si>
+    <t>Square nut</t>
+  </si>
+  <si>
+    <t>Ball bearing</t>
+  </si>
+  <si>
+    <t>Groove ball bearing</t>
+  </si>
+  <si>
+    <t>Flat head hex screw</t>
+  </si>
+  <si>
+    <t>Socket head hex screw</t>
+  </si>
+  <si>
+    <t>Set screw</t>
+  </si>
+  <si>
+    <t>Hex bolt</t>
+  </si>
+  <si>
+    <t>Hex nut</t>
+  </si>
+  <si>
+    <t>Flanged ball bearing</t>
+  </si>
+  <si>
+    <t>https://www.robotshop.com/en/herkulex-drs-0101-robot-servo.html</t>
+  </si>
+  <si>
+    <t>Synchronous pulley T2.5 - Z16</t>
+  </si>
+  <si>
+    <t>Synchronous pulley T5 - Z16 -10mm</t>
+  </si>
+  <si>
+    <t>Synchronous pulley T5 - Z16 -16mm</t>
+  </si>
+  <si>
+    <t>Synchronous pulley T25_z44</t>
+  </si>
+  <si>
+    <t>Synchronous pulley T5_z48</t>
+  </si>
+  <si>
+    <t>Toothed belt T2,5 - Z127  - L317.5mm</t>
+  </si>
+  <si>
+    <t>Spacer M3x5mm</t>
+  </si>
+  <si>
+    <t>Spacer M4x20mm</t>
+  </si>
+  <si>
+    <t>Encoder cap</t>
+  </si>
+  <si>
+    <t>Toothed belt T2,5 - Z80  - L200mm</t>
+  </si>
+  <si>
+    <t>Toothed belt T5 - Z100 - L500mm - 16mm</t>
+  </si>
+  <si>
+    <t>Toothed belt T5 - Z102  - L510mm</t>
+  </si>
+  <si>
+    <t>Toothed belt T5 - Z126 - L630mm</t>
+  </si>
+  <si>
+    <t>Toothed belt T5 - Z68  - L340</t>
+  </si>
+  <si>
+    <t>Encoder - clear</t>
+  </si>
+  <si>
+    <t>Encoder Magnet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -970,32 +1125,69 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H111" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:H111"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Part Name"/>
+    <tableColumn id="2" name="BOM Type"/>
+    <tableColumn id="3" name="Quantity"/>
+    <tableColumn id="4" name="Description"/>
+    <tableColumn id="5" name="Filename"/>
+    <tableColumn id="6" name="Material"/>
+    <tableColumn id="7" name="Estimated Cost" dataDxfId="2"/>
+    <tableColumn id="8" name="Mass (kg)" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1033,9 +1225,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1070,7 +1262,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1105,7 +1297,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1281,11 +1473,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.140625" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
@@ -3734,4 +3926,2454 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="111.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" t="s">
+        <v>311</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.14099999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" t="s">
+        <v>311</v>
+      </c>
+      <c r="H3" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" t="s">
+        <v>311</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" t="s">
+        <v>311</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.70699999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" t="s">
+        <v>311</v>
+      </c>
+      <c r="H6" s="2">
+        <v>7.6999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F7" t="s">
+        <v>311</v>
+      </c>
+      <c r="H7" s="2">
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" t="s">
+        <v>311</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F9" t="s">
+        <v>311</v>
+      </c>
+      <c r="H9" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>200</v>
+      </c>
+      <c r="F10" t="s">
+        <v>311</v>
+      </c>
+      <c r="H10" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>201</v>
+      </c>
+      <c r="F11" t="s">
+        <v>311</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F12" t="s">
+        <v>311</v>
+      </c>
+      <c r="H12" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>238</v>
+      </c>
+      <c r="F13" t="s">
+        <v>311</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>208</v>
+      </c>
+      <c r="F14" t="s">
+        <v>311</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>214</v>
+      </c>
+      <c r="F15" t="s">
+        <v>311</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>215</v>
+      </c>
+      <c r="F16" t="s">
+        <v>311</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" t="s">
+        <v>216</v>
+      </c>
+      <c r="F17" t="s">
+        <v>311</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>213</v>
+      </c>
+      <c r="F18" t="s">
+        <v>311</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>217</v>
+      </c>
+      <c r="F19" t="s">
+        <v>311</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>239</v>
+      </c>
+      <c r="F20" t="s">
+        <v>311</v>
+      </c>
+      <c r="H20" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>240</v>
+      </c>
+      <c r="F21" t="s">
+        <v>311</v>
+      </c>
+      <c r="H21" s="2">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>218</v>
+      </c>
+      <c r="F22" t="s">
+        <v>311</v>
+      </c>
+      <c r="H22" s="2">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" t="s">
+        <v>219</v>
+      </c>
+      <c r="F23" t="s">
+        <v>311</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F24" t="s">
+        <v>311</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>241</v>
+      </c>
+      <c r="F25" t="s">
+        <v>311</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>242</v>
+      </c>
+      <c r="F26" t="s">
+        <v>311</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0.28399999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" t="s">
+        <v>231</v>
+      </c>
+      <c r="F27" t="s">
+        <v>311</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0.23599999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>232</v>
+      </c>
+      <c r="F28" t="s">
+        <v>311</v>
+      </c>
+      <c r="H28" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>229</v>
+      </c>
+      <c r="F29" t="s">
+        <v>311</v>
+      </c>
+      <c r="H29" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>230</v>
+      </c>
+      <c r="F30" t="s">
+        <v>311</v>
+      </c>
+      <c r="H30" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>352</v>
+      </c>
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>236</v>
+      </c>
+      <c r="F31" t="s">
+        <v>311</v>
+      </c>
+      <c r="H31" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" t="s">
+        <v>310</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>134</v>
+      </c>
+      <c r="E32" t="s">
+        <v>211</v>
+      </c>
+      <c r="F32" t="s">
+        <v>312</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0.159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" t="s">
+        <v>244</v>
+      </c>
+      <c r="H33" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" t="s">
+        <v>244</v>
+      </c>
+      <c r="H34" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>338</v>
+      </c>
+      <c r="B35" t="s">
+        <v>310</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>220</v>
+      </c>
+      <c r="F35" t="s">
+        <v>244</v>
+      </c>
+      <c r="H35" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>339</v>
+      </c>
+      <c r="B36" t="s">
+        <v>310</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" t="s">
+        <v>222</v>
+      </c>
+      <c r="F36" t="s">
+        <v>244</v>
+      </c>
+      <c r="H36" s="2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>340</v>
+      </c>
+      <c r="B37" t="s">
+        <v>310</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>223</v>
+      </c>
+      <c r="F37" t="s">
+        <v>244</v>
+      </c>
+      <c r="H37" s="2">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>341</v>
+      </c>
+      <c r="B38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38" t="s">
+        <v>224</v>
+      </c>
+      <c r="F38" t="s">
+        <v>244</v>
+      </c>
+      <c r="H38" s="2">
+        <v>2.955E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>342</v>
+      </c>
+      <c r="B39" t="s">
+        <v>310</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" t="s">
+        <v>225</v>
+      </c>
+      <c r="F39" t="s">
+        <v>244</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>228</v>
+      </c>
+      <c r="F40" t="s">
+        <v>314</v>
+      </c>
+      <c r="H40" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" t="s">
+        <v>310</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>325</v>
+      </c>
+      <c r="E41" t="s">
+        <v>203</v>
+      </c>
+      <c r="F41" t="s">
+        <v>313</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" t="s">
+        <v>310</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>325</v>
+      </c>
+      <c r="E42" t="s">
+        <v>204</v>
+      </c>
+      <c r="F42" t="s">
+        <v>313</v>
+      </c>
+      <c r="H42" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
+        <v>310</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>133</v>
+      </c>
+      <c r="E43" t="s">
+        <v>209</v>
+      </c>
+      <c r="F43" t="s">
+        <v>312</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" t="s">
+        <v>310</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44" t="s">
+        <v>210</v>
+      </c>
+      <c r="F44" t="s">
+        <v>312</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" t="s">
+        <v>310</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" t="s">
+        <v>195</v>
+      </c>
+      <c r="F45" t="s">
+        <v>315</v>
+      </c>
+      <c r="H45" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" t="s">
+        <v>310</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" t="s">
+        <v>196</v>
+      </c>
+      <c r="F46" t="s">
+        <v>315</v>
+      </c>
+      <c r="H46" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>343</v>
+      </c>
+      <c r="B47" t="s">
+        <v>310</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>233</v>
+      </c>
+      <c r="F47" t="s">
+        <v>315</v>
+      </c>
+      <c r="H47" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" t="s">
+        <v>119</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>227</v>
+      </c>
+      <c r="F48" t="s">
+        <v>321</v>
+      </c>
+      <c r="H48" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>344</v>
+      </c>
+      <c r="B49" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>191</v>
+      </c>
+      <c r="F49" t="s">
+        <v>322</v>
+      </c>
+      <c r="H49" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>345</v>
+      </c>
+      <c r="B50" t="s">
+        <v>310</v>
+      </c>
+      <c r="C50">
+        <v>31</v>
+      </c>
+      <c r="E50" t="s">
+        <v>192</v>
+      </c>
+      <c r="F50" t="s">
+        <v>322</v>
+      </c>
+      <c r="H50" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>346</v>
+      </c>
+      <c r="B51" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>237</v>
+      </c>
+      <c r="F51" t="s">
+        <v>323</v>
+      </c>
+      <c r="H51" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>347</v>
+      </c>
+      <c r="B52" t="s">
+        <v>310</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52" t="s">
+        <v>258</v>
+      </c>
+      <c r="H52" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>348</v>
+      </c>
+      <c r="B53" t="s">
+        <v>310</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>234</v>
+      </c>
+      <c r="F53" t="s">
+        <v>258</v>
+      </c>
+      <c r="H53" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>349</v>
+      </c>
+      <c r="B54" t="s">
+        <v>310</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>234</v>
+      </c>
+      <c r="F54" t="s">
+        <v>258</v>
+      </c>
+      <c r="H54" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>350</v>
+      </c>
+      <c r="B55" t="s">
+        <v>310</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>234</v>
+      </c>
+      <c r="F55" t="s">
+        <v>258</v>
+      </c>
+      <c r="H55" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>351</v>
+      </c>
+      <c r="B56" t="s">
+        <v>310</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>118</v>
+      </c>
+      <c r="F56" t="s">
+        <v>258</v>
+      </c>
+      <c r="H56" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" t="s">
+        <v>310</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>326</v>
+      </c>
+      <c r="E57" t="s">
+        <v>205</v>
+      </c>
+      <c r="F57" t="s">
+        <v>255</v>
+      </c>
+      <c r="H57" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" t="s">
+        <v>310</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>326</v>
+      </c>
+      <c r="E58" t="s">
+        <v>206</v>
+      </c>
+      <c r="F58" t="s">
+        <v>255</v>
+      </c>
+      <c r="H58" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" t="s">
+        <v>310</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" t="s">
+        <v>212</v>
+      </c>
+      <c r="F59" t="s">
+        <v>312</v>
+      </c>
+      <c r="H59" s="2">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>353</v>
+      </c>
+      <c r="B60" t="s">
+        <v>310</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>198</v>
+      </c>
+      <c r="F60" t="s">
+        <v>324</v>
+      </c>
+      <c r="H60" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>310</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>327</v>
+      </c>
+      <c r="E61" t="s">
+        <v>145</v>
+      </c>
+      <c r="F61" t="s">
+        <v>255</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" t="s">
+        <v>310</v>
+      </c>
+      <c r="C62">
+        <v>68</v>
+      </c>
+      <c r="D62" t="s">
+        <v>327</v>
+      </c>
+      <c r="E62" t="s">
+        <v>146</v>
+      </c>
+      <c r="F62" t="s">
+        <v>255</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>310</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>327</v>
+      </c>
+      <c r="E63" t="s">
+        <v>147</v>
+      </c>
+      <c r="F63" t="s">
+        <v>255</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" t="s">
+        <v>310</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>327</v>
+      </c>
+      <c r="E64" t="s">
+        <v>148</v>
+      </c>
+      <c r="F64" t="s">
+        <v>255</v>
+      </c>
+      <c r="H64" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>18</v>
+      </c>
+      <c r="B65" t="s">
+        <v>310</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>327</v>
+      </c>
+      <c r="E65" t="s">
+        <v>149</v>
+      </c>
+      <c r="F65" t="s">
+        <v>255</v>
+      </c>
+      <c r="H65" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" t="s">
+        <v>310</v>
+      </c>
+      <c r="C66">
+        <v>13</v>
+      </c>
+      <c r="D66" t="s">
+        <v>328</v>
+      </c>
+      <c r="E66" t="s">
+        <v>150</v>
+      </c>
+      <c r="F66" t="s">
+        <v>255</v>
+      </c>
+      <c r="H66" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
+        <v>310</v>
+      </c>
+      <c r="C67">
+        <v>11</v>
+      </c>
+      <c r="D67" t="s">
+        <v>329</v>
+      </c>
+      <c r="E67" t="s">
+        <v>151</v>
+      </c>
+      <c r="F67" t="s">
+        <v>255</v>
+      </c>
+      <c r="H67" s="2">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" t="s">
+        <v>310</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>329</v>
+      </c>
+      <c r="E68" t="s">
+        <v>152</v>
+      </c>
+      <c r="F68" t="s">
+        <v>255</v>
+      </c>
+      <c r="H68" s="2">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" t="s">
+        <v>310</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>329</v>
+      </c>
+      <c r="E69" t="s">
+        <v>153</v>
+      </c>
+      <c r="F69" t="s">
+        <v>255</v>
+      </c>
+      <c r="H69" s="2">
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" t="s">
+        <v>310</v>
+      </c>
+      <c r="C70">
+        <v>12</v>
+      </c>
+      <c r="D70" t="s">
+        <v>329</v>
+      </c>
+      <c r="E70" t="s">
+        <v>154</v>
+      </c>
+      <c r="F70" t="s">
+        <v>255</v>
+      </c>
+      <c r="H70" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B71" t="s">
+        <v>310</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>329</v>
+      </c>
+      <c r="E71" t="s">
+        <v>155</v>
+      </c>
+      <c r="F71" t="s">
+        <v>255</v>
+      </c>
+      <c r="H71" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72" t="s">
+        <v>310</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>330</v>
+      </c>
+      <c r="E72" t="s">
+        <v>156</v>
+      </c>
+      <c r="F72" t="s">
+        <v>255</v>
+      </c>
+      <c r="H72" s="2">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>26</v>
+      </c>
+      <c r="B73" t="s">
+        <v>310</v>
+      </c>
+      <c r="C73">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>330</v>
+      </c>
+      <c r="E73" t="s">
+        <v>157</v>
+      </c>
+      <c r="F73" t="s">
+        <v>255</v>
+      </c>
+      <c r="H73" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" t="s">
+        <v>310</v>
+      </c>
+      <c r="C74">
+        <v>12</v>
+      </c>
+      <c r="D74" t="s">
+        <v>331</v>
+      </c>
+      <c r="E74" t="s">
+        <v>158</v>
+      </c>
+      <c r="F74" t="s">
+        <v>255</v>
+      </c>
+      <c r="H74" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>28</v>
+      </c>
+      <c r="B75" t="s">
+        <v>310</v>
+      </c>
+      <c r="C75">
+        <v>4</v>
+      </c>
+      <c r="D75" t="s">
+        <v>331</v>
+      </c>
+      <c r="E75" t="s">
+        <v>159</v>
+      </c>
+      <c r="F75" t="s">
+        <v>255</v>
+      </c>
+      <c r="H75" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>29</v>
+      </c>
+      <c r="B76" t="s">
+        <v>310</v>
+      </c>
+      <c r="C76">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
+        <v>331</v>
+      </c>
+      <c r="E76" t="s">
+        <v>160</v>
+      </c>
+      <c r="F76" t="s">
+        <v>255</v>
+      </c>
+      <c r="H76" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s">
+        <v>310</v>
+      </c>
+      <c r="C77">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>331</v>
+      </c>
+      <c r="E77" t="s">
+        <v>161</v>
+      </c>
+      <c r="F77" t="s">
+        <v>255</v>
+      </c>
+      <c r="H77" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" t="s">
+        <v>310</v>
+      </c>
+      <c r="C78">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
+        <v>331</v>
+      </c>
+      <c r="E78" t="s">
+        <v>162</v>
+      </c>
+      <c r="F78" t="s">
+        <v>255</v>
+      </c>
+      <c r="H78" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>32</v>
+      </c>
+      <c r="B79" t="s">
+        <v>310</v>
+      </c>
+      <c r="C79">
+        <v>18</v>
+      </c>
+      <c r="D79" t="s">
+        <v>327</v>
+      </c>
+      <c r="E79" t="s">
+        <v>163</v>
+      </c>
+      <c r="F79" t="s">
+        <v>255</v>
+      </c>
+      <c r="H79" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>33</v>
+      </c>
+      <c r="B80" t="s">
+        <v>310</v>
+      </c>
+      <c r="C80">
+        <v>6</v>
+      </c>
+      <c r="D80" t="s">
+        <v>332</v>
+      </c>
+      <c r="E80" t="s">
+        <v>164</v>
+      </c>
+      <c r="F80" t="s">
+        <v>255</v>
+      </c>
+      <c r="H80" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" t="s">
+        <v>310</v>
+      </c>
+      <c r="C81">
+        <v>12</v>
+      </c>
+      <c r="D81" t="s">
+        <v>332</v>
+      </c>
+      <c r="E81" t="s">
+        <v>165</v>
+      </c>
+      <c r="F81" t="s">
+        <v>255</v>
+      </c>
+      <c r="H81" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" t="s">
+        <v>310</v>
+      </c>
+      <c r="C82">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>332</v>
+      </c>
+      <c r="E82" t="s">
+        <v>166</v>
+      </c>
+      <c r="F82" t="s">
+        <v>255</v>
+      </c>
+      <c r="H82" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83" t="s">
+        <v>310</v>
+      </c>
+      <c r="C83">
+        <v>3</v>
+      </c>
+      <c r="D83" t="s">
+        <v>332</v>
+      </c>
+      <c r="E83" t="s">
+        <v>167</v>
+      </c>
+      <c r="F83" t="s">
+        <v>255</v>
+      </c>
+      <c r="H83" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" t="s">
+        <v>310</v>
+      </c>
+      <c r="C84">
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>332</v>
+      </c>
+      <c r="E84" t="s">
+        <v>168</v>
+      </c>
+      <c r="F84" t="s">
+        <v>255</v>
+      </c>
+      <c r="H84" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>38</v>
+      </c>
+      <c r="B85" t="s">
+        <v>310</v>
+      </c>
+      <c r="C85">
+        <v>26</v>
+      </c>
+      <c r="D85" t="s">
+        <v>332</v>
+      </c>
+      <c r="E85" t="s">
+        <v>169</v>
+      </c>
+      <c r="F85" t="s">
+        <v>255</v>
+      </c>
+      <c r="H85" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>39</v>
+      </c>
+      <c r="B86" t="s">
+        <v>310</v>
+      </c>
+      <c r="C86">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>332</v>
+      </c>
+      <c r="E86" t="s">
+        <v>170</v>
+      </c>
+      <c r="F86" t="s">
+        <v>255</v>
+      </c>
+      <c r="H86" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" t="s">
+        <v>310</v>
+      </c>
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87" t="s">
+        <v>332</v>
+      </c>
+      <c r="E87" t="s">
+        <v>171</v>
+      </c>
+      <c r="F87" t="s">
+        <v>255</v>
+      </c>
+      <c r="H87" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>41</v>
+      </c>
+      <c r="B88" t="s">
+        <v>310</v>
+      </c>
+      <c r="C88">
+        <v>10</v>
+      </c>
+      <c r="D88" t="s">
+        <v>332</v>
+      </c>
+      <c r="E88" t="s">
+        <v>172</v>
+      </c>
+      <c r="F88" t="s">
+        <v>255</v>
+      </c>
+      <c r="H88" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>42</v>
+      </c>
+      <c r="B89" t="s">
+        <v>310</v>
+      </c>
+      <c r="C89">
+        <v>19</v>
+      </c>
+      <c r="D89" t="s">
+        <v>332</v>
+      </c>
+      <c r="E89" t="s">
+        <v>173</v>
+      </c>
+      <c r="F89" t="s">
+        <v>255</v>
+      </c>
+      <c r="H89" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>43</v>
+      </c>
+      <c r="B90" t="s">
+        <v>310</v>
+      </c>
+      <c r="C90">
+        <v>5</v>
+      </c>
+      <c r="D90" t="s">
+        <v>332</v>
+      </c>
+      <c r="E90" t="s">
+        <v>174</v>
+      </c>
+      <c r="F90" t="s">
+        <v>255</v>
+      </c>
+      <c r="H90" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>44</v>
+      </c>
+      <c r="B91" t="s">
+        <v>310</v>
+      </c>
+      <c r="C91">
+        <v>18</v>
+      </c>
+      <c r="D91" t="s">
+        <v>332</v>
+      </c>
+      <c r="E91" t="s">
+        <v>175</v>
+      </c>
+      <c r="F91" t="s">
+        <v>255</v>
+      </c>
+      <c r="H91" s="2">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>45</v>
+      </c>
+      <c r="B92" t="s">
+        <v>310</v>
+      </c>
+      <c r="C92">
+        <v>6</v>
+      </c>
+      <c r="D92" t="s">
+        <v>333</v>
+      </c>
+      <c r="E92" t="s">
+        <v>176</v>
+      </c>
+      <c r="F92" t="s">
+        <v>255</v>
+      </c>
+      <c r="H92" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93" t="s">
+        <v>310</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
+        <v>333</v>
+      </c>
+      <c r="E93" t="s">
+        <v>177</v>
+      </c>
+      <c r="F93" t="s">
+        <v>255</v>
+      </c>
+      <c r="H93" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>47</v>
+      </c>
+      <c r="B94" t="s">
+        <v>310</v>
+      </c>
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s">
+        <v>333</v>
+      </c>
+      <c r="E94" t="s">
+        <v>178</v>
+      </c>
+      <c r="F94" t="s">
+        <v>255</v>
+      </c>
+      <c r="H94" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>48</v>
+      </c>
+      <c r="B95" t="s">
+        <v>310</v>
+      </c>
+      <c r="C95">
+        <v>7</v>
+      </c>
+      <c r="D95" t="s">
+        <v>333</v>
+      </c>
+      <c r="E95" t="s">
+        <v>179</v>
+      </c>
+      <c r="F95" t="s">
+        <v>255</v>
+      </c>
+      <c r="H95" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>49</v>
+      </c>
+      <c r="B96" t="s">
+        <v>310</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>333</v>
+      </c>
+      <c r="E96" t="s">
+        <v>180</v>
+      </c>
+      <c r="F96" t="s">
+        <v>255</v>
+      </c>
+      <c r="H96" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>50</v>
+      </c>
+      <c r="B97" t="s">
+        <v>310</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>334</v>
+      </c>
+      <c r="E97" t="s">
+        <v>181</v>
+      </c>
+      <c r="F97" t="s">
+        <v>255</v>
+      </c>
+      <c r="H97" s="2">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>51</v>
+      </c>
+      <c r="B98" t="s">
+        <v>310</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>334</v>
+      </c>
+      <c r="E98" t="s">
+        <v>182</v>
+      </c>
+      <c r="F98" t="s">
+        <v>255</v>
+      </c>
+      <c r="H98" s="2">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>52</v>
+      </c>
+      <c r="B99" t="s">
+        <v>310</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99" t="s">
+        <v>334</v>
+      </c>
+      <c r="E99" t="s">
+        <v>183</v>
+      </c>
+      <c r="F99" t="s">
+        <v>255</v>
+      </c>
+      <c r="H99" s="2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" t="s">
+        <v>310</v>
+      </c>
+      <c r="C100">
+        <v>4</v>
+      </c>
+      <c r="D100" t="s">
+        <v>334</v>
+      </c>
+      <c r="E100" t="s">
+        <v>184</v>
+      </c>
+      <c r="F100" t="s">
+        <v>255</v>
+      </c>
+      <c r="H100" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>54</v>
+      </c>
+      <c r="B101" t="s">
+        <v>310</v>
+      </c>
+      <c r="C101">
+        <v>6</v>
+      </c>
+      <c r="D101" t="s">
+        <v>334</v>
+      </c>
+      <c r="E101" t="s">
+        <v>185</v>
+      </c>
+      <c r="F101" t="s">
+        <v>255</v>
+      </c>
+      <c r="H101" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>55</v>
+      </c>
+      <c r="B102" t="s">
+        <v>310</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s">
+        <v>334</v>
+      </c>
+      <c r="E102" t="s">
+        <v>186</v>
+      </c>
+      <c r="F102" t="s">
+        <v>255</v>
+      </c>
+      <c r="H102" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>56</v>
+      </c>
+      <c r="B103" t="s">
+        <v>310</v>
+      </c>
+      <c r="C103">
+        <v>10</v>
+      </c>
+      <c r="D103" t="s">
+        <v>335</v>
+      </c>
+      <c r="E103" t="s">
+        <v>187</v>
+      </c>
+      <c r="F103" t="s">
+        <v>255</v>
+      </c>
+      <c r="H103" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>57</v>
+      </c>
+      <c r="B104" t="s">
+        <v>310</v>
+      </c>
+      <c r="C104">
+        <v>53</v>
+      </c>
+      <c r="D104" t="s">
+        <v>335</v>
+      </c>
+      <c r="E104" t="s">
+        <v>188</v>
+      </c>
+      <c r="F104" t="s">
+        <v>255</v>
+      </c>
+      <c r="H104" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>58</v>
+      </c>
+      <c r="B105" t="s">
+        <v>310</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>335</v>
+      </c>
+      <c r="E105" t="s">
+        <v>189</v>
+      </c>
+      <c r="F105" t="s">
+        <v>255</v>
+      </c>
+      <c r="H105" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>59</v>
+      </c>
+      <c r="B106" t="s">
+        <v>310</v>
+      </c>
+      <c r="C106">
+        <v>3</v>
+      </c>
+      <c r="D106" t="s">
+        <v>335</v>
+      </c>
+      <c r="E106" t="s">
+        <v>190</v>
+      </c>
+      <c r="F106" t="s">
+        <v>255</v>
+      </c>
+      <c r="H106" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>68</v>
+      </c>
+      <c r="B107" t="s">
+        <v>310</v>
+      </c>
+      <c r="C107">
+        <v>11</v>
+      </c>
+      <c r="D107" t="s">
+        <v>336</v>
+      </c>
+      <c r="E107" t="s">
+        <v>199</v>
+      </c>
+      <c r="F107" t="s">
+        <v>255</v>
+      </c>
+      <c r="H107" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>95</v>
+      </c>
+      <c r="B108" t="s">
+        <v>119</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="E108" t="s">
+        <v>226</v>
+      </c>
+      <c r="F108" t="s">
+        <v>255</v>
+      </c>
+      <c r="H108" s="2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>97</v>
+      </c>
+      <c r="B109" t="s">
+        <v>119</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="E109" t="s">
+        <v>226</v>
+      </c>
+      <c r="F109" t="s">
+        <v>255</v>
+      </c>
+      <c r="H109" s="2">
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>98</v>
+      </c>
+      <c r="B110" t="s">
+        <v>119</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="E110" t="s">
+        <v>226</v>
+      </c>
+      <c r="F110" t="s">
+        <v>255</v>
+      </c>
+      <c r="H110" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+      <c r="B111" t="s">
+        <v>310</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="E111" t="s">
+        <v>235</v>
+      </c>
+      <c r="F111" t="s">
+        <v>312</v>
+      </c>
+      <c r="H111" s="2">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D111" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>